<commit_message>
refactor: simplify and clean up schema focused on BDF tools
</commit_message>
<xml_diff>
--- a/project/excel/bdf_toolbox_schema.xlsx
+++ b/project/excel/bdf_toolbox_schema.xlsx
@@ -451,7 +451,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -462,44 +462,37 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>primary_email</t>
+          <t>developer_team</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>birth_date</t>
+          <t>technical_area</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>age_in_years</t>
+          <t>id</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>vital_status</t>
+          <t>name</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"ALIVE,DEAD,UNKNOWN"</formula1>
+  <dataValidations count="2">
+    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"ASKEM_NEU,ASKEM_MIT,ASKEM_NYU,ASKEM_Jataware,Netrias,N3C,BDC,CRA,DNAHIVE,HMS,Stanford,UAB,ICF,SageBio,Insilicom"</formula1>
+    </dataValidation>
+    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"TA1,TA2,TA3"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
feat: add keywords and url to tool schema
</commit_message>
<xml_diff>
--- a/project/excel/bdf_toolbox_schema.xlsx
+++ b/project/excel/bdf_toolbox_schema.xlsx
@@ -451,7 +451,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -472,15 +472,25 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
+          <t>keywords</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>url</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>description</t>
         </is>

</xml_diff>